<commit_message>
Adding charts in excel
</commit_message>
<xml_diff>
--- a/heap_sort_analysis.xlsx
+++ b/heap_sort_analysis.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545"/>
+    <workbookView xWindow="4360" yWindow="980" windowWidth="21560" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -27,17 +32,20 @@
     <t>time spent (s)</t>
   </si>
   <si>
-    <t>sift down</t>
+    <t>SIFT UP</t>
   </si>
   <si>
-    <t>sift up</t>
+    <t>SIFT DOWN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +53,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -62,20 +106,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -83,6 +219,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:C8" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9">
+  <autoFilter ref="A4:C8"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="k" dataDxfId="3"/>
+    <tableColumn id="2" name="comparisons" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="time spent (s)" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="E4:G8" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
+  <autoFilter ref="E4:G8"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="k" dataDxfId="5"/>
+    <tableColumn id="2" name="comparisons" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="time spent (s)" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,137 +532,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="16.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="6" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="2" spans="1:8">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
         <v>469</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C5" s="1">
         <v>1.4E-5</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F5" s="2">
         <v>2315</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G5" s="1">
         <v>6.7000000000000002E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="2">
         <v>8095</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C6" s="1">
         <v>1.7100000000000001E-4</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F6" s="2">
         <v>207084</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G6" s="1">
         <v>7.9620000000000003E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7" s="2">
         <v>114247</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C7" s="1">
         <v>2.362E-3</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E7" s="1">
         <v>4</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F7" s="2">
         <v>19205574</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G7" s="1">
         <v>0.72317900000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B8" s="2">
         <v>1474588</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C8" s="1">
         <v>3.5684E-2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E8" s="1">
         <v>5</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F8" s="2">
         <v>1942533363</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G8" s="1">
         <v>52.985242999999997</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -512,9 +699,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -524,8 +716,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>